<commit_message>
fixed scaling on data collection
</commit_message>
<xml_diff>
--- a/Lab9/Data Collection (Nyquist).xlsx
+++ b/Lab9/Data Collection (Nyquist).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Documents\EE445L\Lab9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FF1366-A649-4613-86BB-C474CF7532B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84542645-A93F-46DA-B795-BCA3A53BBAE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{89B434D1-7521-4DE4-ADD5-2F21C5DAF805}"/>
   </bookViews>
@@ -538,7 +538,6 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -556,6 +555,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -600,6 +654,8 @@
         <c:axId val="558705904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -617,6 +673,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ADC</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Value</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1169,6 +1285,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Samples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1213,6 +1384,8 @@
         <c:axId val="560473656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1230,6 +1403,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ADC Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1782,6 +2010,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sample</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1826,6 +2109,8 @@
         <c:axId val="565821944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1843,6 +2128,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ADC</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3608,16 +3952,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3644,16 +3988,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:rowOff>130175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3680,16 +4024,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4014,18 +4358,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918D2620-A24F-4FF3-9DDF-F00CF1070891}">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4035,11 +4376,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>998</v>
       </c>
@@ -4050,7 +4391,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1336</v>
       </c>
@@ -4061,7 +4402,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1886</v>
       </c>
@@ -4072,7 +4413,7 @@
         <v>2726</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2434</v>
       </c>
@@ -4083,7 +4424,7 @@
         <v>2725</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2769</v>
       </c>
@@ -4094,7 +4435,7 @@
         <v>2730</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2771</v>
       </c>
@@ -4105,7 +4446,7 @@
         <v>2721</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2430</v>
       </c>
@@ -4116,7 +4457,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1878</v>
       </c>
@@ -4127,7 +4468,7 @@
         <v>2724</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1339</v>
       </c>
@@ -4138,7 +4479,7 @@
         <v>2723</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>998</v>
       </c>
@@ -4149,7 +4490,7 @@
         <v>2728</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>998</v>
       </c>
@@ -4160,7 +4501,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1334</v>
       </c>
@@ -4171,7 +4512,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1883</v>
       </c>
@@ -4182,7 +4523,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2440</v>
       </c>
@@ -4193,7 +4534,7 @@
         <v>2732</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2774</v>
       </c>

</xml_diff>